<commit_message>
Primer push del proyecto castela_nueva
</commit_message>
<xml_diff>
--- a/cuasinoides.xlsx
+++ b/cuasinoides.xlsx
@@ -2918,8 +2918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DT25"/>
   <sheetViews>
-    <sheetView topLeftCell="N4" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:U25"/>
+    <sheetView topLeftCell="BL1" workbookViewId="0">
+      <selection activeCell="BT1" sqref="BT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12286,8 +12286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX25"/>
   <sheetViews>
-    <sheetView topLeftCell="O4" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1:AC25"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16101,8 +16101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JS25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" topLeftCell="GT1" workbookViewId="0">
+      <selection activeCell="GU1" sqref="GU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>